<commit_message>
admin console CRUD operations works
</commit_message>
<xml_diff>
--- a/sql/SqlDescription.xlsx
+++ b/sql/SqlDescription.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Event" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -38,6 +39,18 @@
   </si>
   <si>
     <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userId(mail)</t>
   </si>
 </sst>
 </file>
@@ -136,14 +149,11 @@
   </sheetPr>
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -198,4 +208,61 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regularna"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>